<commit_message>
Update Design Report and Sprints
Scrum updates and Report updates
</commit_message>
<xml_diff>
--- a/Scrum/CST361-SprintBurnDown Milestone 1.xlsx
+++ b/Scrum/CST361-SprintBurnDown Milestone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachs\OneDrive\Documents\GitHub\CST361Group\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0430BFD6-8350-4024-8A75-C08A5B6729DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30636776-7638-465A-A0CB-FC71A3307078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1413,7 +1413,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,6 +2511,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9FDC2B66788A044965A7B8958E6244A" ma:contentTypeVersion="1252" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b057034aaaed5c863779c49b233863c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d6188da8-f31e-469a-aed4-03a23c44e36a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1c6f164606e2683634ad95dba38a1a4a" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2705,39 +2723,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B9AF611-705C-4987-B883-1E6816B1C18B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D99B8B-5BC3-4C4D-8BB2-30740DC6BB75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="d6188da8-f31e-469a-aed4-03a23c44e36a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2760,9 +2749,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D99B8B-5BC3-4C4D-8BB2-30740DC6BB75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B9AF611-705C-4987-B883-1E6816B1C18B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="d6188da8-f31e-469a-aed4-03a23c44e36a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>